<commit_message>
feat: Make for placement test certificate
</commit_message>
<xml_diff>
--- a/public/examples/graduation_example.xlsx
+++ b/public/examples/graduation_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27911"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oak Soe Aung\Development\projects\KBTC-Assets\Graduation\InternationalSchool\ExcelFormats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OakSoeAung\Development\Work\kbtc\ExamResult\public\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1D5B51-F3C9-457B-9481-84EC15406EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAFF784-1099-4FA6-9EAF-63A20F7EE551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2198D89A-5D40-429D-941B-B07BF447D3F0}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>English</t>
   </si>
@@ -65,24 +64,15 @@
     <t>Biology</t>
   </si>
   <si>
-    <t>He consistently demonstrates a strong work ethic and a genuine passion for learning.</t>
-  </si>
-  <si>
     <t>zawlinkyaw</t>
   </si>
   <si>
     <t>Information</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>Mr Oak Soe Aung</t>
   </si>
   <si>
-    <t>Remark of the Class Teacher</t>
-  </si>
-  <si>
     <t>Student ID</t>
   </si>
   <si>
@@ -99,9 +89,6 @@
   </si>
   <si>
     <t>KBTC-STD-1000</t>
-  </si>
-  <si>
-    <t>Class Teacher Sign</t>
   </si>
   <si>
     <t>Mark</t>
@@ -157,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,12 +169,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7E5E4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,22 +182,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A21A16A-CC1A-4C34-B273-1A840106E98A}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,33 +564,31 @@
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>6</v>
@@ -625,93 +600,83 @@
         <v>8</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="10"/>
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
+      <c r="I2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <v>36590</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1">
         <v>45544</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>90</v>
@@ -737,17 +702,10 @@
       <c r="P3" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>